<commit_message>
excel com coimbra privado atualizado
</commit_message>
<xml_diff>
--- a/VLSM_Subnet.xlsx
+++ b/VLSM_Subnet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rribe\GNS3\projects\trabalhoED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D88EEEC-9746-41BD-A007-D8D2957BE6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238FF7AC-293F-4087-A829-1484DC38A9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6A4E2B9A-4F10-42F5-BB30-E89D31521063}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" xr2:uid="{6A4E2B9A-4F10-42F5-BB30-E89D31521063}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="244">
   <si>
     <t>Hosts Needed</t>
   </si>
@@ -732,16 +732,40 @@
     <t>Coimbra</t>
   </si>
   <si>
-    <t xml:space="preserve">? </t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>VLSM p/ cada filial. Ips públicos</t>
   </si>
   <si>
     <t>Subnet p/cada filial. Ips privados</t>
+  </si>
+  <si>
+    <t>192.168.1.32 - 192.168.1.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.33 - 192.168.1.46 </t>
+  </si>
+  <si>
+    <t>Coimbra B</t>
+  </si>
+  <si>
+    <t>192.168.1.48 - 192.168.1.51</t>
+  </si>
+  <si>
+    <t>192.168.1.49 - 192.168.1.50</t>
+  </si>
+  <si>
+    <t>Coimbra C</t>
+  </si>
+  <si>
+    <t>/30</t>
+  </si>
+  <si>
+    <t>192.168.1.52 - 192.168.1.55</t>
+  </si>
+  <si>
+    <t>192.168.1.53 - 192.168.1.54</t>
+  </si>
+  <si>
+    <t>Ligações entre routers que meti lá paraas áreas</t>
   </si>
 </sst>
 </file>
@@ -857,7 +881,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -977,11 +1001,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1112,6 +1145,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1435,41 +1474,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D075DA04-2DD1-4762-85E5-45D9155CE74B}">
-  <dimension ref="B1:Q56"/>
+  <dimension ref="B1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
     <col min="15" max="15" width="35.5703125" customWidth="1"/>
     <col min="16" max="16" width="34.28515625" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F1" s="42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
       <c r="O1" s="42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P1" s="44"/>
     </row>
-    <row r="3" spans="2:17" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>216</v>
       </c>
@@ -1514,7 +1554,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1549,16 +1589,16 @@
         <v>231</v>
       </c>
       <c r="O4" s="37" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="P4" s="37" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="Q4" s="37" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1589,20 +1629,27 @@
       <c r="K5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="O5" s="40" t="s">
-        <v>220</v>
-      </c>
-      <c r="P5" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q5" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="N5" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="R5" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+    </row>
+    <row r="6" spans="2:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1633,20 +1680,25 @@
       <c r="K6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="O6" s="40" t="s">
-        <v>223</v>
-      </c>
-      <c r="P6" s="40" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q6" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="N6" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="R6" s="45"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+    </row>
+    <row r="7" spans="2:22" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1677,20 +1729,20 @@
       <c r="K7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="34" t="s">
-        <v>225</v>
+      <c r="N7" s="32" t="s">
+        <v>215</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="P7" s="40" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="Q7" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1721,20 +1773,20 @@
       <c r="K8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="O8" s="41" t="s">
-        <v>229</v>
+      <c r="N8" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="O8" s="40" t="s">
+        <v>223</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="Q8" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1765,8 +1817,20 @@
       <c r="K9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="N9" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="O9" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="P9" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q9" s="40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1797,8 +1861,20 @@
       <c r="K10" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="N10" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="P10" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q10" s="40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1830,7 +1906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>44</v>
       </c>
@@ -1862,7 +1938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:17" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
         <v>48</v>
       </c>
@@ -1894,7 +1970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
         <v>52</v>
       </c>
@@ -1926,7 +2002,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>59</v>
       </c>
@@ -1958,7 +2034,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>63</v>
       </c>
@@ -1990,7 +2066,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>67</v>
       </c>
@@ -2022,7 +2098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>71</v>
       </c>
@@ -2054,7 +2130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>75</v>
       </c>
@@ -2086,7 +2162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>79</v>
       </c>
@@ -2118,7 +2194,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>83</v>
       </c>
@@ -2150,7 +2226,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>87</v>
       </c>
@@ -2182,7 +2258,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>91</v>
       </c>
@@ -2214,7 +2290,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>95</v>
       </c>
@@ -2246,7 +2322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>99</v>
       </c>
@@ -2278,7 +2354,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
         <v>103</v>
       </c>
@@ -2310,7 +2386,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
         <v>107</v>
       </c>
@@ -2342,7 +2418,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
         <v>111</v>
       </c>
@@ -2374,7 +2450,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
         <v>115</v>
       </c>
@@ -2406,7 +2482,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
         <v>119</v>
       </c>
@@ -2438,7 +2514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
         <v>123</v>
       </c>
@@ -2470,7 +2546,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
         <v>127</v>
       </c>
@@ -2502,7 +2578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>131</v>
       </c>
@@ -2534,7 +2610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
         <v>135</v>
       </c>
@@ -2566,7 +2642,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
         <v>139</v>
       </c>
@@ -2598,7 +2674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
         <v>143</v>
       </c>
@@ -2630,7 +2706,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>147</v>
       </c>
@@ -2662,7 +2738,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
         <v>151</v>
       </c>
@@ -2694,7 +2770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
         <v>155</v>
       </c>
@@ -2726,7 +2802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
         <v>159</v>
       </c>
@@ -2758,7 +2834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
         <v>163</v>
       </c>
@@ -2790,7 +2866,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B42" s="22" t="s">
         <v>167</v>
       </c>
@@ -2822,7 +2898,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
         <v>171</v>
       </c>
@@ -2854,7 +2930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B44" s="24" t="s">
         <v>175</v>
       </c>
@@ -2886,7 +2962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
         <v>179</v>
       </c>
@@ -2918,7 +2994,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B46" s="25" t="s">
         <v>183</v>
       </c>
@@ -2950,7 +3026,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B47" s="25" t="s">
         <v>187</v>
       </c>
@@ -2982,7 +3058,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
         <v>191</v>
       </c>
@@ -3014,7 +3090,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B49" s="25" t="s">
         <v>195</v>
       </c>
@@ -3046,7 +3122,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B50" s="25" t="s">
         <v>199</v>
       </c>
@@ -3078,7 +3154,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B51" s="25" t="s">
         <v>203</v>
       </c>
@@ -3110,7 +3186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B52" s="26" t="s">
         <v>207</v>
       </c>
@@ -3142,7 +3218,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="27" t="s">
         <v>211</v>
       </c>
@@ -3178,9 +3254,10 @@
       <c r="B56" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R5:V6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>